<commit_message>
added a bunch of changes
</commit_message>
<xml_diff>
--- a/StudentProfile.xlsx
+++ b/StudentProfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F84E3E3-1A87-8A46-8301-F65766DD5FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB6E9CB-E19B-794C-9BF4-2C8DC12D7986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
   </bookViews>
@@ -244,22 +244,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">High School Year attended: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(e.g. Sophomore Year)</t>
-    </r>
-  </si>
-  <si>
     <t>Positive Personality Traits (Please select up to 6):</t>
   </si>
   <si>
@@ -318,9 +302,6 @@
     <t>2021/2022</t>
   </si>
   <si>
-    <t>Junior Year</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -328,6 +309,25 @@
   </si>
   <si>
     <t>Other(type here)</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">High School Year attended: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(e.g. Sophomore)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
   <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -775,12 +775,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,15 +796,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,15 +820,15 @@
         <v>56</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -837,44 +837,44 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="9"/>
     </row>
@@ -889,7 +889,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" s="9"/>
     </row>
@@ -924,7 +924,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -937,7 +937,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -951,7 +951,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -971,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>14</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
         <v>18</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>26</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>29</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
         <v>31</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
         <v>34</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,13 +1158,13 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B61" s="9"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>46</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
         <v>48</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>50</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1259,7 +1259,7 @@
         <v>52</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B80" s="9"/>
     </row>

</xml_diff>

<commit_message>
wrapping up for the day, it is midnight
</commit_message>
<xml_diff>
--- a/StudentProfile.xlsx
+++ b/StudentProfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEFA378-EE7B-324A-80B8-64EA615287F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8EE046-5324-9D4A-8345-C4D767A7A61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>First Name:</t>
   </si>
@@ -293,6 +293,9 @@
     <t>AP Environmental Science</t>
   </si>
   <si>
+    <t>2021/2022</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
@@ -319,6 +322,9 @@
       </rPr>
       <t>(e.g. Sophomore)</t>
     </r>
+  </si>
+  <si>
+    <t>2018/2019</t>
   </si>
   <si>
     <t>2020/2021</t>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF65202-81E2-7743-AF86-81EEEFE6CD76}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -773,23 +779,23 @@
     <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="34.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="1.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -797,7 +803,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -805,7 +811,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
@@ -813,7 +819,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>55</v>
       </c>
@@ -821,70 +827,79 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B14" s="9"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="9"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" s="9"/>
     </row>
@@ -899,7 +914,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -907,7 +922,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -924,7 +939,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" s="9"/>
     </row>
@@ -947,7 +962,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -955,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -963,7 +978,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -971,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -979,7 +994,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,7 +1002,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1160,7 +1175,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B61" s="9"/>
     </row>
@@ -1191,7 +1206,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1205,7 +1220,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1234,7 @@
         <v>46</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1233,7 +1248,7 @@
         <v>48</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1247,7 +1262,7 @@
         <v>50</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,7 +1276,7 @@
         <v>52</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1287,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B80" s="9"/>
     </row>

</xml_diff>

<commit_message>
More text were added to the dicctionaries
</commit_message>
<xml_diff>
--- a/StudentProfile.xlsx
+++ b/StudentProfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8EE046-5324-9D4A-8345-C4D767A7A61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804E3F10-DBB1-2141-BE31-131CA012CCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,12 +284,6 @@
     <t>Scholarship Program</t>
   </si>
   <si>
-    <t>Anand</t>
-  </si>
-  <si>
-    <t>Pranav</t>
-  </si>
-  <si>
     <t>AP Environmental Science</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
   </si>
   <si>
     <t>Other(type here)</t>
-  </si>
-  <si>
-    <t>Junior</t>
   </si>
   <si>
     <r>
@@ -330,9 +321,6 @@
     <t>2020/2021</t>
   </si>
   <si>
-    <t>Targetted Institution</t>
-  </si>
-  <si>
     <t>James E. Roberts Engineering</t>
   </si>
   <si>
@@ -340,6 +328,31 @@
   </si>
   <si>
     <t>University</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Targetted Institution </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(e.g MIT)</t>
+    </r>
+  </si>
+  <si>
+    <t>Chicão</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t>Science Mater Tow</t>
   </si>
 </sst>
 </file>
@@ -769,7 +782,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -800,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -808,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -824,7 +837,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,24 +845,24 @@
         <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -857,7 +870,7 @@
         <v>77</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -868,7 +881,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -879,15 +892,15 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B14" s="9"/>
     </row>
@@ -899,7 +912,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B16" s="9"/>
     </row>
@@ -914,7 +927,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +935,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +952,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="9"/>
     </row>
@@ -962,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +983,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -978,7 +991,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -986,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1002,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1175,7 +1188,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B61" s="9"/>
     </row>
@@ -1206,7 +1219,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1233,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1234,7 +1247,7 @@
         <v>46</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1248,7 +1261,7 @@
         <v>48</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,7 +1275,7 @@
         <v>50</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1276,7 +1289,7 @@
         <v>52</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1287,7 +1300,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B80" s="9"/>
     </row>

</xml_diff>

<commit_message>
Minor fixes and added details to readme
</commit_message>
<xml_diff>
--- a/StudentProfile.xlsx
+++ b/StudentProfile.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D1D350-CC14-2C45-87A7-5C4F450F8529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C0F27-0E9F-D845-BA32-5D4852EE9E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Profile" sheetId="1" r:id="rId1"/>
+    <sheet name="DB" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="trais" localSheetId="1">DB!$A$1:$B$54</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,8 +38,21 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{90A4ADFB-D23A-FC49-84DE-F31391476C33}" name="trais" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr sourceFile="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/trais.txt" tab="0" delimiter=":">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="116">
   <si>
     <t>First Name:</t>
   </si>
@@ -312,9 +329,6 @@
     <t>University</t>
   </si>
   <si>
-    <t>she</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Targetted Institution </t>
     </r>
@@ -331,18 +345,6 @@
     </r>
   </si>
   <si>
-    <t>Senior</t>
-  </si>
-  <si>
-    <t>Amanda</t>
-  </si>
-  <si>
-    <t>Freitag</t>
-  </si>
-  <si>
-    <t>UC Berkeley</t>
-  </si>
-  <si>
     <t>&lt;- Please Write it here</t>
   </si>
   <si>
@@ -356,6 +358,123 @@
   </si>
   <si>
     <t>&lt;- Please Mark with X which ones apply</t>
+  </si>
+  <si>
+    <t>PositivePersonalityTraits</t>
+  </si>
+  <si>
+    <t>dedicates a lof of time helping others</t>
+  </si>
+  <si>
+    <t>is always friendly and pleasant with me and the other students</t>
+  </si>
+  <si>
+    <t>frequently demonstrates the ability to speak fluently and coherently</t>
+  </si>
+  <si>
+    <t>is exceptionally clever and talented always striving for the best results</t>
+  </si>
+  <si>
+    <t>is very quick at learning new concepts and ideas</t>
+  </si>
+  <si>
+    <t>dedicates a lot of time to study always aiming to achieve good grades and be in the top of the class</t>
+  </si>
+  <si>
+    <t>delivers homework and assignments in time, very deserving of trust</t>
+  </si>
+  <si>
+    <t>shows determination to get things done not allowing any difficulties get in the way</t>
+  </si>
+  <si>
+    <t>shows intense interest for our class activities and concepts that we learn in class</t>
+  </si>
+  <si>
+    <t>reacts well to set backs and is able to adapt to new situations quickly</t>
+  </si>
+  <si>
+    <t>gives full attention during lectures and class activities, avoiding distractions</t>
+  </si>
+  <si>
+    <t>shares knowledge with other students and makes sure classmates are participating and learning the material as well</t>
+  </si>
+  <si>
+    <t>admits own actions and share sincere opinions and ideas without being hurtful</t>
+  </si>
+  <si>
+    <t>make sure other students are also participating in activities and help to organize the classroom</t>
+  </si>
+  <si>
+    <t>AcademicSkills</t>
+  </si>
+  <si>
+    <t>even in the face of adversity, puts a lot of commitment to honesty, trust, fairness, respect, responsibility, and courage</t>
+  </si>
+  <si>
+    <t>is exceptionally clever and talented, always striving for the best results</t>
+  </si>
+  <si>
+    <t>dedicates a lot of time to study, always aiming to achieve good grades and be in the top of the class</t>
+  </si>
+  <si>
+    <t>participates in all individual and group activities and discussions</t>
+  </si>
+  <si>
+    <t>has the the ability to handle difficult or unexpected situations, finding more than one solution to a problem</t>
+  </si>
+  <si>
+    <t>is motivated to get things done, always presenting a lot of enthusiasm and interest on studies or projects without needing pressure</t>
+  </si>
+  <si>
+    <t>is a a person who strives to do the best for the team, always at ease while working with other students, co-operating with them, whenever leading or taking instructions from others</t>
+  </si>
+  <si>
+    <t>is very goal oriented, likes to serve others and take the lead into projects or stepping-up as a team leader while in class</t>
+  </si>
+  <si>
+    <t>even in the face of adversity, is highly adaptable to the new environment, demonstrating a lot of flexibility and ability to cope with change with grace</t>
+  </si>
+  <si>
+    <t>is very diligent in laboring and puts a lot of effort into doing and completing tasks, including homework, projects, and participating in class activities</t>
+  </si>
+  <si>
+    <t>has the ability to solve problems or tasks in a creative way, by means of generating many original ideas, carrying distictive cognitive traits and nonconformist behavior</t>
+  </si>
+  <si>
+    <t>constantly demonstrates having the ability to use various concepts with their meanings, to make inferences by making suggestions and to make reasoning by focusing on problem solving based on logical thinking</t>
+  </si>
+  <si>
+    <t>has the ability to deliver information to different kinds of audiences in an effective and engaging manner</t>
+  </si>
+  <si>
+    <t>gets high marks and good grades. Usually goes beyond the work that is required and does it very well. Usually the work is well-organized, neat and delivered on time</t>
+  </si>
+  <si>
+    <t>is always very confident when answering questions</t>
+  </si>
+  <si>
+    <t>is a big picture thinker, asks a lot of good questions making connections with other facts and tries to learn a lot about the subject</t>
+  </si>
+  <si>
+    <t>is very indulgent, considerate and always providing help to whoever is in need</t>
+  </si>
+  <si>
+    <t>enjoys applying logical reasoning to solve problems, is very data driven and adepts at recognizing patterns</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Horseshik</t>
+  </si>
+  <si>
+    <t>Myassis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -486,6 +605,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="trais" connectionId="1" xr16:uid="{D863A13F-6A68-8144-BEAC-4B29DB6D4415}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF65202-81E2-7743-AF86-81EEEFE6CD76}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -806,15 +929,15 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -822,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,7 +953,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -839,7 +962,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -857,7 +980,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="2" t="s">
@@ -875,16 +998,16 @@
         <v>66</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -901,7 +1024,7 @@
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,9 +1038,7 @@
       <c r="A14" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B14" s="9"/>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,7 +1052,9 @@
       <c r="A16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +1077,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -995,7 +1118,7 @@
         <v>64</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1018,9 +1141,7 @@
       <c r="A30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B30" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -1054,7 +1175,9 @@
       <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="9"/>
+      <c r="B35" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -1226,7 +1349,7 @@
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1329,4 +1452,369 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35C1360-9693-9748-9CDB-F352101AFB89}">
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView zoomScale="161" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="178.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Limited the number of Skills and traits
</commit_message>
<xml_diff>
--- a/StudentProfile.xlsx
+++ b/StudentProfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C0F27-0E9F-D845-BA32-5D4852EE9E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09BACC6-48D0-AA41-9620-34901EC26B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="116">
   <si>
     <t>First Name:</t>
   </si>
@@ -468,13 +468,13 @@
     <t>Junior</t>
   </si>
   <si>
-    <t>Horseshik</t>
-  </si>
-  <si>
-    <t>Myassis</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Trei</t>
+  </si>
+  <si>
+    <t>Tulia</t>
+  </si>
+  <si>
+    <t>MIT</t>
   </si>
 </sst>
 </file>
@@ -568,17 +568,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -910,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF65202-81E2-7743-AF86-81EEEFE6CD76}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -928,7 +926,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>72</v>
       </c>
     </row>
@@ -936,7 +934,7 @@
       <c r="A2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -944,7 +942,7 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>113</v>
       </c>
     </row>
@@ -952,37 +950,37 @@
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
         <v>67</v>
       </c>
@@ -997,86 +995,84 @@
       <c r="A8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1084,23 +1080,19 @@
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1108,16 +1100,14 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="10" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1125,7 +1115,7 @@
       <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1133,207 +1123,203 @@
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B31" s="7"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="7"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B35" s="7"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="9"/>
+      <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="9"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="9"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="9"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="9"/>
+      <c r="B41" s="7"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="7"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="9"/>
+      <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="9"/>
+      <c r="B44" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="9"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="9"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="9"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="9"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="9"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="9"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="9"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="9"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B55" s="9"/>
+      <c r="B55" s="7"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B56" s="9"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="9"/>
+      <c r="B57" s="7"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="9"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="9"/>
+      <c r="B59" s="7"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="9"/>
+      <c r="B60" s="7"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="9"/>
+      <c r="B61" s="7"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -1341,14 +1327,14 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+      <c r="A65" s="5"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="12" t="s">
+      <c r="B66" s="7"/>
+      <c r="C66" s="10" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1356,13 +1342,13 @@
       <c r="A67" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B67" s="9"/>
+      <c r="B67" s="7"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1370,69 +1356,63 @@
       <c r="A69" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B69" s="9"/>
+      <c r="B69" s="7"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B70" s="7"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B71" s="9"/>
+      <c r="B71" s="7"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B72" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B72" s="7"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B73" s="9"/>
+      <c r="B73" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B74" s="7"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B75" s="9"/>
+      <c r="B75" s="7"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B76" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="B76" s="7"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B77" s="9"/>
+      <c r="B77" s="7"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1440,13 +1420,13 @@
       <c r="A79" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B79" s="9"/>
+      <c r="B79" s="7"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B80" s="9"/>
+      <c r="B80" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed an issue when no instituition is required
</commit_message>
<xml_diff>
--- a/StudentProfile.xlsx
+++ b/StudentProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clfilho/Dropbox (Personal)/Rec-Auto/Python Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09BACC6-48D0-AA41-9620-34901EC26B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD75FA87-E99B-2745-8583-17A07C52F8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
+    <workbookView xWindow="-37080" yWindow="460" windowWidth="33600" windowHeight="20500" xr2:uid="{8A1CF855-2C5B-F149-936A-A90AA29A5A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Profile" sheetId="1" r:id="rId1"/>
@@ -23,16 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -468,10 +458,10 @@
     <t>Junior</t>
   </si>
   <si>
-    <t>Trei</t>
-  </si>
-  <si>
-    <t>Tulia</t>
+    <t>Abeer</t>
+  </si>
+  <si>
+    <t>Bajpai</t>
   </si>
   <si>
     <t>MIT</t>
@@ -909,7 +899,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1069,9 +1059,7 @@
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="10" t="s">
         <v>75</v>
       </c>
@@ -1080,7 +1068,9 @@
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1141,7 +1131,9 @@
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -1165,9 +1157,7 @@
       <c r="A36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="B36" s="7"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -1362,7 +1352,9 @@
       <c r="A70" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="7"/>
+      <c r="B70" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
@@ -1412,9 +1404,7 @@
       <c r="A78" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="B78" s="7"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">

</xml_diff>